<commit_message>
[IMP] Temporary save 20221028
</commit_message>
<xml_diff>
--- a/assets_management/data/example.xlsx
+++ b/assets_management/data/example.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Completo #1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Totale+Svalutazione" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Parziale" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Completo #2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Totale+Svalutazione" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Parziale" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="45">
   <si>
     <t xml:space="preserve">Descrizione</t>
   </si>
@@ -394,11 +395,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="10.39"/>
@@ -1164,6 +1165,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="true" objects="true" scenarios="true"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1179,13 +1181,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ49"/>
+  <dimension ref="A1:AMJ48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="10.39"/>
@@ -1218,18 +1220,18 @@
         <v>4</v>
       </c>
       <c r="B2" s="4" t="n">
-        <v>1000</v>
+        <v>2500</v>
       </c>
       <c r="C2" s="5" t="n">
         <f aca="false">B2</f>
-        <v>1000</v>
+        <v>2500</v>
       </c>
       <c r="D2" s="6"/>
       <c r="F2" s="0" t="s">
         <v>5</v>
       </c>
       <c r="G2" s="7" t="n">
-        <v>0.25</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1237,7 +1239,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="8" t="n">
-        <v>183</v>
+        <v>92</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>7</v>
@@ -1247,7 +1249,7 @@
       </c>
       <c r="G3" s="6" t="n">
         <f aca="false">$B$2*G2</f>
-        <v>250</v>
+        <v>600</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1256,11 +1258,11 @@
       </c>
       <c r="B4" s="5" t="n">
         <f aca="false">$G$3*B3/366</f>
-        <v>125</v>
+        <v>150.819672131148</v>
       </c>
       <c r="C4" s="5" t="n">
         <f aca="false">C2-B4</f>
-        <v>875</v>
+        <v>2349.18032786885</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="0" t="s">
@@ -1275,467 +1277,481 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" s="8" t="n">
-        <v>31</v>
-      </c>
-      <c r="C5" s="5"/>
+        <v>12</v>
+      </c>
+      <c r="B5" s="5" t="n">
+        <f aca="false">$G$3</f>
+        <v>600</v>
+      </c>
+      <c r="C5" s="5" t="n">
+        <f aca="false">C4-B5</f>
+        <v>1749.18032786885</v>
+      </c>
       <c r="D5" s="6"/>
-      <c r="G5" s="9"/>
+      <c r="E5" s="0" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="5" t="n">
-        <f aca="false">$G$3*B5/365</f>
-        <v>21.2328767123288</v>
-      </c>
-      <c r="C6" s="5" t="n">
-        <f aca="false">C4-B6</f>
-        <v>853.767123287671</v>
-      </c>
-      <c r="D6" s="6"/>
+        <v>14</v>
+      </c>
+      <c r="B6" s="8" t="n">
+        <v>31</v>
+      </c>
       <c r="E6" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="8" t="n">
-        <v>31</v>
+        <v>16</v>
+      </c>
+      <c r="B7" s="5" t="n">
+        <f aca="false">$G$3*B6/365</f>
+        <v>50.958904109589</v>
+      </c>
+      <c r="C7" s="5" t="n">
+        <f aca="false">C5-B7</f>
+        <v>1698.22142375926</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B8" s="5" t="n">
-        <f aca="false">$G$3*B7/365</f>
-        <v>21.2328767123288</v>
+        <f aca="false">C7*$G$4</f>
+        <v>1698.22142375926</v>
       </c>
       <c r="C8" s="5" t="n">
-        <f aca="false">C6-B8</f>
-        <v>832.534246575342</v>
+        <f aca="false">C7-B8</f>
+        <v>0</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="5" t="n">
-        <f aca="false">C8*$G$4</f>
-        <v>832.534246575342</v>
-      </c>
-      <c r="C9" s="5" t="n">
-        <f aca="false">C8-B9</f>
-        <v>0</v>
+        <v>19</v>
+      </c>
+      <c r="B9" s="4" t="n">
+        <v>3210</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="4" t="n">
-        <v>1400</v>
+        <v>21</v>
+      </c>
+      <c r="B10" s="5" t="n">
+        <f aca="false">B9-B8</f>
+        <v>1511.77857624074</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="5" t="n">
-        <f aca="false">B10-B9</f>
-        <v>567.465753424658</v>
-      </c>
-      <c r="E11" s="0" t="s">
         <v>22</v>
       </c>
     </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D12" s="6"/>
+    </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D13" s="6"/>
+      <c r="A13" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="F14" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="G14" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="H14" s="0" t="s">
-        <v>26</v>
+      <c r="E14" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14" s="6" t="n">
+        <f aca="false">$B$2</f>
+        <v>2500</v>
+      </c>
+      <c r="H14" s="6" t="n">
+        <f aca="false">F14-G14</f>
+        <v>-2500</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>28</v>
+      </c>
       <c r="E15" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="G15" s="6" t="n">
+        <v>29</v>
+      </c>
+      <c r="F15" s="6" t="n">
         <f aca="false">$B$2</f>
-        <v>1000</v>
+        <v>2500</v>
       </c>
       <c r="H15" s="6" t="n">
         <f aca="false">F15-G15</f>
-        <v>-1000</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
+      </c>
+      <c r="C16" s="6" t="n">
+        <f aca="false">B4</f>
+        <v>150.819672131148</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="F16" s="6" t="n">
-        <f aca="false">$B$2</f>
-        <v>1000</v>
+        <v>30</v>
+      </c>
+      <c r="G16" s="6" t="n">
+        <f aca="false">C16</f>
+        <v>150.819672131148</v>
       </c>
       <c r="H16" s="6" t="n">
         <f aca="false">F16-G16</f>
-        <v>1000</v>
+        <v>-150.819672131148</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="6" t="n">
+        <v>31</v>
+      </c>
+      <c r="B17" s="5" t="n">
         <f aca="false">B4</f>
-        <v>125</v>
+        <v>150.819672131148</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="G17" s="6" t="n">
-        <f aca="false">C17</f>
-        <v>125</v>
+        <v>32</v>
+      </c>
+      <c r="F17" s="6" t="n">
+        <f aca="false">B17</f>
+        <v>150.819672131148</v>
       </c>
       <c r="H17" s="6" t="n">
         <f aca="false">F17-G17</f>
-        <v>-125</v>
+        <v>150.819672131148</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" s="5" t="n">
-        <f aca="false">B4</f>
-        <v>125</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="F18" s="6" t="n">
-        <f aca="false">B18</f>
-        <v>125</v>
-      </c>
-      <c r="H18" s="6" t="n">
-        <f aca="false">F18-G18</f>
-        <v>125</v>
+      <c r="A18" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="11" t="n">
+        <f aca="false">SUM(B15:B17)</f>
+        <v>150.819672131148</v>
+      </c>
+      <c r="C18" s="11" t="n">
+        <f aca="false">SUM(C15:C17)</f>
+        <v>150.819672131148</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H18" s="2" t="n">
+        <f aca="false">H15+H16</f>
+        <v>2349.18032786885</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" s="11" t="n">
-        <f aca="false">SUM(B16:B18)</f>
-        <v>125</v>
-      </c>
-      <c r="C19" s="11" t="n">
-        <f aca="false">SUM(C16:C18)</f>
-        <v>125</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H19" s="2" t="n">
-        <f aca="false">H16+H17</f>
-        <v>875</v>
-      </c>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
+      <c r="A20" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" s="6" t="n">
+        <f aca="false">$B$2</f>
+        <v>2500</v>
+      </c>
+      <c r="H20" s="6" t="n">
+        <f aca="false">F20-G20</f>
+        <v>2500</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>35</v>
+        <v>30</v>
+      </c>
+      <c r="C21" s="6" t="n">
+        <f aca="false">B5</f>
+        <v>600</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="F21" s="6" t="n">
-        <f aca="false">$B$2</f>
-        <v>1000</v>
+        <v>30</v>
+      </c>
+      <c r="G21" s="6" t="n">
+        <f aca="false">G16+C21</f>
+        <v>750.819672131148</v>
       </c>
       <c r="H21" s="6" t="n">
         <f aca="false">F21-G21</f>
-        <v>1000</v>
+        <v>-750.819672131148</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22" s="6" t="n">
-        <f aca="false">B6</f>
-        <v>21.2328767123288</v>
+        <v>31</v>
+      </c>
+      <c r="B22" s="5" t="n">
+        <f aca="false">B5</f>
+        <v>600</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="G22" s="6" t="n">
-        <f aca="false">G17+C22</f>
-        <v>146.232876712329</v>
+        <v>32</v>
+      </c>
+      <c r="F22" s="6" t="n">
+        <f aca="false">B22</f>
+        <v>600</v>
       </c>
       <c r="H22" s="6" t="n">
         <f aca="false">F22-G22</f>
-        <v>-146.232876712329</v>
+        <v>600</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23" s="5" t="n">
-        <f aca="false">B6</f>
-        <v>21.2328767123288</v>
-      </c>
-      <c r="E23" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="F23" s="6" t="n">
-        <f aca="false">B23</f>
-        <v>21.2328767123288</v>
-      </c>
-      <c r="H23" s="6" t="n">
-        <f aca="false">F23-G23</f>
-        <v>21.2328767123288</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="10" t="s">
+      <c r="A23" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B24" s="11" t="n">
-        <f aca="false">SUM(B21:B23)</f>
-        <v>21.2328767123288</v>
-      </c>
-      <c r="C24" s="11" t="n">
-        <f aca="false">SUM(C21:C23)</f>
-        <v>21.2328767123288</v>
-      </c>
-      <c r="E24" s="1" t="s">
+      <c r="B23" s="11" t="n">
+        <f aca="false">SUM(B20:B22)</f>
+        <v>600</v>
+      </c>
+      <c r="C23" s="11" t="n">
+        <f aca="false">SUM(C20:C22)</f>
+        <v>600</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H24" s="2" t="n">
-        <f aca="false">H21+H22</f>
-        <v>853.767123287671</v>
+      <c r="H23" s="2" t="n">
+        <f aca="false">H20+H21</f>
+        <v>1749.18032786885</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F25" s="6" t="n">
+        <f aca="false">$B$2</f>
+        <v>2500</v>
+      </c>
+      <c r="H25" s="6" t="n">
+        <f aca="false">F25-G25</f>
+        <v>2500</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>36</v>
+        <v>30</v>
+      </c>
+      <c r="C26" s="6" t="n">
+        <f aca="false">B7</f>
+        <v>50.958904109589</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="F26" s="6" t="n">
-        <f aca="false">$B$2</f>
-        <v>1000</v>
+        <v>30</v>
+      </c>
+      <c r="G26" s="6" t="n">
+        <f aca="false">G21+C26</f>
+        <v>801.778576240737</v>
       </c>
       <c r="H26" s="6" t="n">
         <f aca="false">F26-G26</f>
-        <v>1000</v>
+        <v>-801.778576240737</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C27" s="6" t="n">
-        <f aca="false">B8</f>
-        <v>21.2328767123288</v>
+        <v>31</v>
+      </c>
+      <c r="B27" s="5" t="n">
+        <f aca="false">B7</f>
+        <v>50.958904109589</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="G27" s="6" t="n">
-        <f aca="false">G22+C27</f>
-        <v>167.465753424658</v>
+        <v>32</v>
+      </c>
+      <c r="F27" s="6" t="n">
+        <f aca="false">B27</f>
+        <v>50.958904109589</v>
       </c>
       <c r="H27" s="6" t="n">
         <f aca="false">F27-G27</f>
-        <v>-167.465753424658</v>
+        <v>50.958904109589</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="B28" s="5" t="n">
-        <f aca="false">B8</f>
-        <v>21.2328767123288</v>
-      </c>
-      <c r="E28" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="F28" s="6" t="n">
-        <f aca="false">B28</f>
-        <v>21.2328767123288</v>
-      </c>
-      <c r="H28" s="6" t="n">
-        <f aca="false">F28-G28</f>
-        <v>21.2328767123288</v>
+      <c r="A28" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="11" t="n">
+        <f aca="false">SUM(B25:B27)</f>
+        <v>50.958904109589</v>
+      </c>
+      <c r="C28" s="11" t="n">
+        <f aca="false">SUM(C25:C27)</f>
+        <v>50.958904109589</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H28" s="2" t="n">
+        <f aca="false">H25+H26</f>
+        <v>1698.22142375926</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B29" s="11" t="n">
-        <f aca="false">SUM(B26:B28)</f>
-        <v>21.2328767123288</v>
-      </c>
-      <c r="C29" s="11" t="n">
-        <f aca="false">SUM(C26:C28)</f>
-        <v>21.2328767123288</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H29" s="2" t="n">
-        <f aca="false">H26+H27</f>
-        <v>832.534246575342</v>
-      </c>
+      <c r="A29" s="10"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="10"/>
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
+      <c r="A30" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F30" s="6" t="n">
+        <f aca="false">$B$2</f>
+        <v>2500</v>
+      </c>
+      <c r="G30" s="6" t="n">
+        <f aca="false">C32</f>
+        <v>3210</v>
+      </c>
+      <c r="H30" s="6" t="n">
+        <f aca="false">F30-G30</f>
+        <v>-710</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>37</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="B31" s="6" t="n">
+        <f aca="false">B9</f>
+        <v>3210</v>
+      </c>
+      <c r="C31" s="6"/>
       <c r="E31" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="F31" s="6" t="n">
-        <f aca="false">$B$2</f>
-        <v>1000</v>
+        <v>30</v>
       </c>
       <c r="G31" s="6" t="n">
-        <f aca="false">C33</f>
-        <v>1400</v>
+        <f aca="false">G26</f>
+        <v>801.778576240737</v>
       </c>
       <c r="H31" s="6" t="n">
         <f aca="false">F31-G31</f>
-        <v>-400</v>
+        <v>-801.778576240737</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="B32" s="6" t="n">
-        <f aca="false">B10</f>
-        <v>1400</v>
-      </c>
-      <c r="C32" s="6"/>
+        <v>29</v>
+      </c>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6" t="n">
+        <f aca="false">B9</f>
+        <v>3210</v>
+      </c>
       <c r="E32" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="G32" s="6" t="n">
-        <f aca="false">G27</f>
-        <v>167.465753424658</v>
+        <v>32</v>
+      </c>
+      <c r="F32" s="6" t="n">
+        <f aca="false">B32</f>
+        <v>0</v>
       </c>
       <c r="H32" s="6" t="n">
         <f aca="false">F32-G32</f>
-        <v>-167.465753424658</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6" t="n">
-        <f aca="false">B10</f>
-        <v>1400</v>
-      </c>
-      <c r="E33" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="F33" s="6" t="n">
-        <f aca="false">B33</f>
-        <v>0</v>
-      </c>
-      <c r="H33" s="6" t="n">
-        <f aca="false">F33-G33</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="10" t="s">
+      <c r="A33" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="11" t="n">
-        <f aca="false">SUM(B31:B33)</f>
-        <v>1400</v>
-      </c>
-      <c r="C34" s="11" t="n">
-        <f aca="false">SUM(C31:C33)</f>
-        <v>1400</v>
-      </c>
-      <c r="E34" s="1" t="s">
+      <c r="B33" s="11" t="n">
+        <f aca="false">SUM(B30:B32)</f>
+        <v>3210</v>
+      </c>
+      <c r="C33" s="11" t="n">
+        <f aca="false">SUM(C30:C32)</f>
+        <v>3210</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H34" s="2" t="n">
-        <f aca="false">H31+H32</f>
-        <v>-567.465753424658</v>
+      <c r="H33" s="2" t="n">
+        <f aca="false">H30+H31</f>
+        <v>-1511.77857624074</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F35" s="6" t="n">
+        <f aca="false">F30+B36</f>
+        <v>3210</v>
+      </c>
+      <c r="G35" s="6" t="n">
+        <f aca="false">G30+C39</f>
+        <v>3210</v>
+      </c>
+      <c r="H35" s="6" t="n">
+        <f aca="false">F35-G35</f>
+        <v>0</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>18</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="B36" s="6" t="n">
+        <f aca="false">B10-G26</f>
+        <v>710</v>
+      </c>
+      <c r="C36" s="6"/>
       <c r="E36" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F36" s="6" t="n">
-        <f aca="false">F31+B37</f>
-        <v>1400</v>
+        <f aca="false">F26+B38</f>
+        <v>801.778576240737</v>
       </c>
       <c r="G36" s="6" t="n">
-        <f aca="false">G31+C40</f>
-        <v>1400</v>
+        <f aca="false">G26</f>
+        <v>801.778576240737</v>
       </c>
       <c r="H36" s="6" t="n">
         <f aca="false">F36-G36</f>
@@ -1744,23 +1760,19 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="B37" s="6" t="n">
-        <f aca="false">B11-G27</f>
-        <v>400</v>
-      </c>
-      <c r="C37" s="6"/>
+        <v>21</v>
+      </c>
+      <c r="B37" s="6"/>
+      <c r="C37" s="5" t="n">
+        <f aca="false">B10</f>
+        <v>1511.77857624074</v>
+      </c>
       <c r="E37" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F37" s="6" t="n">
-        <f aca="false">F27+B39</f>
-        <v>167.465753424658</v>
-      </c>
-      <c r="G37" s="6" t="n">
-        <f aca="false">G27</f>
-        <v>167.465753424658</v>
+        <f aca="false">B37</f>
+        <v>0</v>
       </c>
       <c r="H37" s="6" t="n">
         <f aca="false">F37-G37</f>
@@ -1769,101 +1781,105 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B38" s="6" t="n">
+        <f aca="false">G26</f>
+        <v>801.778576240737</v>
+      </c>
+      <c r="C38" s="6"/>
+      <c r="E38" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="B38" s="6"/>
-      <c r="C38" s="5" t="n">
-        <f aca="false">B11</f>
-        <v>567.465753424658</v>
-      </c>
-      <c r="E38" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="F38" s="6" t="n">
-        <f aca="false">B38</f>
-        <v>0</v>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6" t="n">
+        <f aca="false">C37</f>
+        <v>1511.77857624074</v>
       </c>
       <c r="H38" s="6" t="n">
         <f aca="false">F38-G38</f>
-        <v>0</v>
+        <v>-1511.77857624074</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="B39" s="6" t="n">
-        <f aca="false">G27</f>
-        <v>167.465753424658</v>
-      </c>
-      <c r="C39" s="6"/>
-      <c r="E39" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6" t="n">
-        <f aca="false">C38</f>
-        <v>567.465753424658</v>
-      </c>
-      <c r="H39" s="6" t="n">
-        <f aca="false">F39-G39</f>
-        <v>-567.465753424658</v>
+        <v>29</v>
+      </c>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H39" s="2" t="n">
+        <f aca="false">H35+H36</f>
+        <v>0</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="B40" s="6"/>
-      <c r="C40" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H40" s="2" t="n">
-        <f aca="false">H36+H37</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="10" t="s">
+      <c r="A40" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B41" s="11" t="n">
-        <f aca="false">SUM(B36:B40)</f>
-        <v>567.465753424658</v>
-      </c>
-      <c r="C41" s="11" t="n">
-        <f aca="false">SUM(C36:C40)</f>
-        <v>567.465753424658</v>
-      </c>
-      <c r="H41" s="6"/>
+      <c r="B40" s="11" t="n">
+        <f aca="false">SUM(B35:B39)</f>
+        <v>1511.77857624074</v>
+      </c>
+      <c r="C40" s="11" t="n">
+        <f aca="false">SUM(C35:C39)</f>
+        <v>1511.77857624074</v>
+      </c>
+      <c r="H40" s="6"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>39</v>
+        <v>29</v>
+      </c>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6" t="n">
+        <f aca="false">C32-B36</f>
+        <v>2500</v>
+      </c>
+      <c r="E43" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F43" s="6" t="n">
+        <f aca="false">F25</f>
+        <v>2500</v>
+      </c>
+      <c r="G43" s="6" t="n">
+        <f aca="false">G25+C43</f>
+        <v>2500</v>
+      </c>
+      <c r="H43" s="6" t="n">
+        <f aca="false">F43-G43</f>
+        <v>0</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B44" s="6"/>
-      <c r="C44" s="6" t="n">
-        <f aca="false">C33-B37</f>
-        <v>1000</v>
+      <c r="C44" s="5" t="n">
+        <f aca="false">C37</f>
+        <v>1511.77857624074</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F44" s="6" t="n">
-        <f aca="false">F26</f>
-        <v>1000</v>
+        <f aca="false">F26+B45</f>
+        <v>801.778576240737</v>
       </c>
       <c r="G44" s="6" t="n">
-        <f aca="false">G26+C44</f>
-        <v>1000</v>
+        <f aca="false">G26</f>
+        <v>801.778576240737</v>
       </c>
       <c r="H44" s="6" t="n">
         <f aca="false">F44-G44</f>
@@ -1872,23 +1888,18 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="B45" s="6"/>
-      <c r="C45" s="5" t="n">
-        <f aca="false">C38</f>
-        <v>567.465753424658</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="B45" s="6" t="n">
+        <f aca="false">B38</f>
+        <v>801.778576240737</v>
+      </c>
+      <c r="C45" s="6"/>
       <c r="E45" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F45" s="6" t="n">
-        <f aca="false">F27+B46</f>
-        <v>167.465753424658</v>
-      </c>
-      <c r="G45" s="6" t="n">
-        <f aca="false">G27</f>
-        <v>167.465753424658</v>
+        <v>0</v>
       </c>
       <c r="H45" s="6" t="n">
         <f aca="false">F45-G45</f>
@@ -1897,71 +1908,52 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="B46" s="6" t="n">
-        <f aca="false">B39</f>
-        <v>167.465753424658</v>
+        <f aca="false">B9</f>
+        <v>3210</v>
       </c>
       <c r="C46" s="6"/>
-      <c r="E46" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="F46" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H46" s="6" t="n">
-        <f aca="false">F46-G46</f>
-        <v>0</v>
-      </c>
+      <c r="F46" s="6"/>
+      <c r="H46" s="6"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="B47" s="6" t="n">
-        <f aca="false">B10</f>
-        <v>1400</v>
-      </c>
-      <c r="C47" s="6"/>
+      <c r="A47" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B47" s="11" t="n">
+        <f aca="false">SUM(B42:B46)</f>
+        <v>4011.77857624074</v>
+      </c>
+      <c r="C47" s="11" t="n">
+        <f aca="false">SUM(C42:C46)</f>
+        <v>4011.77857624074</v>
+      </c>
+      <c r="E47" s="0" t="s">
+        <v>21</v>
+      </c>
       <c r="F47" s="6"/>
-      <c r="H47" s="6"/>
+      <c r="G47" s="6" t="n">
+        <f aca="false">C44</f>
+        <v>1511.77857624074</v>
+      </c>
+      <c r="H47" s="6" t="n">
+        <f aca="false">F47-G47</f>
+        <v>-1511.77857624074</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B48" s="11" t="n">
-        <f aca="false">SUM(B43:B47)</f>
-        <v>1567.46575342466</v>
-      </c>
-      <c r="C48" s="11" t="n">
-        <f aca="false">SUM(C43:C47)</f>
-        <v>1567.46575342466</v>
-      </c>
-      <c r="E48" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="F48" s="6"/>
-      <c r="G48" s="6" t="n">
-        <f aca="false">C45</f>
-        <v>567.465753424658</v>
-      </c>
-      <c r="H48" s="6" t="n">
-        <f aca="false">F48-G48</f>
-        <v>-567.465753424658</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E49" s="1" t="s">
+      <c r="E48" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H49" s="2" t="n">
-        <f aca="false">H44+H45</f>
+      <c r="H48" s="2" t="n">
+        <f aca="false">H43+H44</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="true" objects="true" scenarios="true"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1977,13 +1969,811 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:AMJ49"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="10.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="47.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.91"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2"/>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="3"/>
+      <c r="AMI1" s="0"/>
+      <c r="AMJ1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="4" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C2" s="5" t="n">
+        <f aca="false">B2</f>
+        <v>1000</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="F2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="7" t="n">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="8" t="n">
+        <v>183</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="6" t="n">
+        <f aca="false">$B$2*G2</f>
+        <v>250</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="5" t="n">
+        <f aca="false">$G$3*B3/366</f>
+        <v>125</v>
+      </c>
+      <c r="C4" s="5" t="n">
+        <f aca="false">C2-B4</f>
+        <v>875</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="6"/>
+      <c r="G5" s="9"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="5" t="n">
+        <f aca="false">$G$3*B5/365</f>
+        <v>21.2328767123288</v>
+      </c>
+      <c r="C6" s="5" t="n">
+        <f aca="false">C4-B6</f>
+        <v>853.767123287671</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="5" t="n">
+        <f aca="false">$G$3*B7/365</f>
+        <v>21.2328767123288</v>
+      </c>
+      <c r="C8" s="5" t="n">
+        <f aca="false">C6-B8</f>
+        <v>832.534246575342</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="5" t="n">
+        <f aca="false">C8*$G$4</f>
+        <v>832.534246575342</v>
+      </c>
+      <c r="C9" s="5" t="n">
+        <f aca="false">C8-B9</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="4" t="n">
+        <v>1400</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="5" t="n">
+        <f aca="false">B10-B9</f>
+        <v>567.465753424658</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D13" s="6"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E15" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="G15" s="6" t="n">
+        <f aca="false">$B$2</f>
+        <v>1000</v>
+      </c>
+      <c r="H15" s="6" t="n">
+        <f aca="false">F15-G15</f>
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" s="6" t="n">
+        <f aca="false">$B$2</f>
+        <v>1000</v>
+      </c>
+      <c r="H16" s="6" t="n">
+        <f aca="false">F16-G16</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="6" t="n">
+        <f aca="false">B4</f>
+        <v>125</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G17" s="6" t="n">
+        <f aca="false">C17</f>
+        <v>125</v>
+      </c>
+      <c r="H17" s="6" t="n">
+        <f aca="false">F17-G17</f>
+        <v>-125</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="5" t="n">
+        <f aca="false">B4</f>
+        <v>125</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" s="6" t="n">
+        <f aca="false">B18</f>
+        <v>125</v>
+      </c>
+      <c r="H18" s="6" t="n">
+        <f aca="false">F18-G18</f>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="11" t="n">
+        <f aca="false">SUM(B16:B18)</f>
+        <v>125</v>
+      </c>
+      <c r="C19" s="11" t="n">
+        <f aca="false">SUM(C16:C18)</f>
+        <v>125</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H19" s="2" t="n">
+        <f aca="false">H16+H17</f>
+        <v>875</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21" s="6" t="n">
+        <f aca="false">$B$2</f>
+        <v>1000</v>
+      </c>
+      <c r="H21" s="6" t="n">
+        <f aca="false">F21-G21</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="6" t="n">
+        <f aca="false">B6</f>
+        <v>21.2328767123288</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G22" s="6" t="n">
+        <f aca="false">G17+C22</f>
+        <v>146.232876712329</v>
+      </c>
+      <c r="H22" s="6" t="n">
+        <f aca="false">F22-G22</f>
+        <v>-146.232876712329</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="5" t="n">
+        <f aca="false">B6</f>
+        <v>21.2328767123288</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" s="6" t="n">
+        <f aca="false">B23</f>
+        <v>21.2328767123288</v>
+      </c>
+      <c r="H23" s="6" t="n">
+        <f aca="false">F23-G23</f>
+        <v>21.2328767123288</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="11" t="n">
+        <f aca="false">SUM(B21:B23)</f>
+        <v>21.2328767123288</v>
+      </c>
+      <c r="C24" s="11" t="n">
+        <f aca="false">SUM(C21:C23)</f>
+        <v>21.2328767123288</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H24" s="2" t="n">
+        <f aca="false">H21+H22</f>
+        <v>853.767123287671</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F26" s="6" t="n">
+        <f aca="false">$B$2</f>
+        <v>1000</v>
+      </c>
+      <c r="H26" s="6" t="n">
+        <f aca="false">F26-G26</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="6" t="n">
+        <f aca="false">B8</f>
+        <v>21.2328767123288</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G27" s="6" t="n">
+        <f aca="false">G22+C27</f>
+        <v>167.465753424658</v>
+      </c>
+      <c r="H27" s="6" t="n">
+        <f aca="false">F27-G27</f>
+        <v>-167.465753424658</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="5" t="n">
+        <f aca="false">B8</f>
+        <v>21.2328767123288</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F28" s="6" t="n">
+        <f aca="false">B28</f>
+        <v>21.2328767123288</v>
+      </c>
+      <c r="H28" s="6" t="n">
+        <f aca="false">F28-G28</f>
+        <v>21.2328767123288</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29" s="11" t="n">
+        <f aca="false">SUM(B26:B28)</f>
+        <v>21.2328767123288</v>
+      </c>
+      <c r="C29" s="11" t="n">
+        <f aca="false">SUM(C26:C28)</f>
+        <v>21.2328767123288</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H29" s="2" t="n">
+        <f aca="false">H26+H27</f>
+        <v>832.534246575342</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="10"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F31" s="6" t="n">
+        <f aca="false">$B$2</f>
+        <v>1000</v>
+      </c>
+      <c r="G31" s="6" t="n">
+        <f aca="false">C33</f>
+        <v>1400</v>
+      </c>
+      <c r="H31" s="6" t="n">
+        <f aca="false">F31-G31</f>
+        <v>-400</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32" s="6" t="n">
+        <f aca="false">B10</f>
+        <v>1400</v>
+      </c>
+      <c r="C32" s="6"/>
+      <c r="E32" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G32" s="6" t="n">
+        <f aca="false">G27</f>
+        <v>167.465753424658</v>
+      </c>
+      <c r="H32" s="6" t="n">
+        <f aca="false">F32-G32</f>
+        <v>-167.465753424658</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6" t="n">
+        <f aca="false">B10</f>
+        <v>1400</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F33" s="6" t="n">
+        <f aca="false">B33</f>
+        <v>0</v>
+      </c>
+      <c r="H33" s="6" t="n">
+        <f aca="false">F33-G33</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" s="11" t="n">
+        <f aca="false">SUM(B31:B33)</f>
+        <v>1400</v>
+      </c>
+      <c r="C34" s="11" t="n">
+        <f aca="false">SUM(C31:C33)</f>
+        <v>1400</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H34" s="2" t="n">
+        <f aca="false">H31+H32</f>
+        <v>-567.465753424658</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F36" s="6" t="n">
+        <f aca="false">F31+B37</f>
+        <v>1400</v>
+      </c>
+      <c r="G36" s="6" t="n">
+        <f aca="false">G31+C40</f>
+        <v>1400</v>
+      </c>
+      <c r="H36" s="6" t="n">
+        <f aca="false">F36-G36</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B37" s="6" t="n">
+        <f aca="false">B11-G27</f>
+        <v>400</v>
+      </c>
+      <c r="C37" s="6"/>
+      <c r="E37" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="F37" s="6" t="n">
+        <f aca="false">F27+B39</f>
+        <v>167.465753424658</v>
+      </c>
+      <c r="G37" s="6" t="n">
+        <f aca="false">G27</f>
+        <v>167.465753424658</v>
+      </c>
+      <c r="H37" s="6" t="n">
+        <f aca="false">F37-G37</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B38" s="6"/>
+      <c r="C38" s="5" t="n">
+        <f aca="false">B11</f>
+        <v>567.465753424658</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F38" s="6" t="n">
+        <f aca="false">B38</f>
+        <v>0</v>
+      </c>
+      <c r="H38" s="6" t="n">
+        <f aca="false">F38-G38</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B39" s="6" t="n">
+        <f aca="false">G27</f>
+        <v>167.465753424658</v>
+      </c>
+      <c r="C39" s="6"/>
+      <c r="E39" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6" t="n">
+        <f aca="false">C38</f>
+        <v>567.465753424658</v>
+      </c>
+      <c r="H39" s="6" t="n">
+        <f aca="false">F39-G39</f>
+        <v>-567.465753424658</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H40" s="2" t="n">
+        <f aca="false">H36+H37</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B41" s="11" t="n">
+        <f aca="false">SUM(B36:B40)</f>
+        <v>567.465753424658</v>
+      </c>
+      <c r="C41" s="11" t="n">
+        <f aca="false">SUM(C36:C40)</f>
+        <v>567.465753424658</v>
+      </c>
+      <c r="H41" s="6"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B44" s="6"/>
+      <c r="C44" s="6" t="n">
+        <f aca="false">C33-B37</f>
+        <v>1000</v>
+      </c>
+      <c r="E44" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F44" s="6" t="n">
+        <f aca="false">F26</f>
+        <v>1000</v>
+      </c>
+      <c r="G44" s="6" t="n">
+        <f aca="false">G26+C44</f>
+        <v>1000</v>
+      </c>
+      <c r="H44" s="6" t="n">
+        <f aca="false">F44-G44</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B45" s="6"/>
+      <c r="C45" s="5" t="n">
+        <f aca="false">C38</f>
+        <v>567.465753424658</v>
+      </c>
+      <c r="E45" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="F45" s="6" t="n">
+        <f aca="false">F27+B46</f>
+        <v>167.465753424658</v>
+      </c>
+      <c r="G45" s="6" t="n">
+        <f aca="false">G27</f>
+        <v>167.465753424658</v>
+      </c>
+      <c r="H45" s="6" t="n">
+        <f aca="false">F45-G45</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B46" s="6" t="n">
+        <f aca="false">B39</f>
+        <v>167.465753424658</v>
+      </c>
+      <c r="C46" s="6"/>
+      <c r="E46" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F46" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H46" s="6" t="n">
+        <f aca="false">F46-G46</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B47" s="6" t="n">
+        <f aca="false">B10</f>
+        <v>1400</v>
+      </c>
+      <c r="C47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="H47" s="6"/>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B48" s="11" t="n">
+        <f aca="false">SUM(B43:B47)</f>
+        <v>1567.46575342466</v>
+      </c>
+      <c r="C48" s="11" t="n">
+        <f aca="false">SUM(C43:C47)</f>
+        <v>1567.46575342466</v>
+      </c>
+      <c r="E48" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6" t="n">
+        <f aca="false">C45</f>
+        <v>567.465753424658</v>
+      </c>
+      <c r="H48" s="6" t="n">
+        <f aca="false">F48-G48</f>
+        <v>-567.465753424658</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E49" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H49" s="2" t="n">
+        <f aca="false">H44+H45</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPagina &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:AMJ48"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I34" activeCellId="0" sqref="I34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="10.39"/>

</xml_diff>

<commit_message>
[IMP] Temporary save 20221029
</commit_message>
<xml_diff>
--- a/assets_management/data/example.xlsx
+++ b/assets_management/data/example.xlsx
@@ -5,13 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Completo #1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Completo #2" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Totale+Svalutazione" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Parziale" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Svalutazione #3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Parziale #4" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="55">
   <si>
     <t xml:space="preserve">Descrizione</t>
   </si>
@@ -106,6 +106,9 @@
     <t xml:space="preserve">Saldo</t>
   </si>
   <si>
+    <t xml:space="preserve">Da calcolo bene</t>
+  </si>
+  <si>
     <t xml:space="preserve">Fornitore</t>
   </si>
   <si>
@@ -148,7 +151,34 @@
     <t xml:space="preserve">Transitorio</t>
   </si>
   <si>
+    <t xml:space="preserve">Valore bene</t>
+  </si>
+  <si>
     <t xml:space="preserve"># giorni 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quota 90 giorni</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Svalutazione</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q.A. dopo svalutaz,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># giorni residui 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QA 2021 residua</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quota 275 giorni</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minusvalenza</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ammortamento 2021 residuo</t>
   </si>
   <si>
     <t xml:space="preserve">Compreso giorno di acquisto (anno 366 giorni)</t>
@@ -164,12 +194,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="[$€-410]\ #,##0.00;[RED]\-[$€-410]\ #,##0.00"/>
     <numFmt numFmtId="166" formatCode="0.00%"/>
+    <numFmt numFmtId="167" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -208,6 +239,60 @@
     <font>
       <i val="true"/>
       <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <u val="single"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <strike val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <strike val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF999999"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF999999"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="8"/>
+      <color rgb="FF999999"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF999999"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -267,7 +352,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -313,6 +398,66 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -374,7 +519,7 @@
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF999999"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
@@ -396,7 +541,7 @@
   <dimension ref="A1:AMJ48"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -592,10 +737,13 @@
       <c r="H13" s="0" t="s">
         <v>26</v>
       </c>
+      <c r="I13" s="0" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E14" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G14" s="6" t="n">
         <f aca="false">$B$2</f>
@@ -608,10 +756,10 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F15" s="6" t="n">
         <f aca="false">$B$2</f>
@@ -624,14 +772,14 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C16" s="6" t="n">
         <f aca="false">B4</f>
         <v>125</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G16" s="6" t="n">
         <f aca="false">C16</f>
@@ -644,14 +792,14 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B17" s="5" t="n">
         <f aca="false">B4</f>
         <v>125</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F17" s="6" t="n">
         <f aca="false">B17</f>
@@ -664,7 +812,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B18" s="11" t="n">
         <f aca="false">SUM(B15:B17)</f>
@@ -675,12 +823,16 @@
         <v>125</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H18" s="2" t="n">
         <f aca="false">H15+H16</f>
         <v>875</v>
       </c>
+      <c r="I18" s="12" t="n">
+        <f aca="false">C4</f>
+        <v>875</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G19" s="6"/>
@@ -688,10 +840,10 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F20" s="6" t="n">
         <f aca="false">$B$2</f>
@@ -704,14 +856,14 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C21" s="6" t="n">
         <f aca="false">B5</f>
         <v>250</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G21" s="6" t="n">
         <f aca="false">G16+C21</f>
@@ -724,14 +876,14 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B22" s="5" t="n">
         <f aca="false">B5</f>
         <v>250</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F22" s="6" t="n">
         <f aca="false">B22</f>
@@ -744,7 +896,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B23" s="11" t="n">
         <f aca="false">SUM(B20:B22)</f>
@@ -755,19 +907,23 @@
         <v>250</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H23" s="2" t="n">
         <f aca="false">H20+H21</f>
         <v>625</v>
       </c>
+      <c r="I23" s="12" t="n">
+        <f aca="false">C5</f>
+        <v>625</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F25" s="6" t="n">
         <f aca="false">$B$2</f>
@@ -780,14 +936,14 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C26" s="6" t="n">
         <f aca="false">B7</f>
         <v>21.2328767123288</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G26" s="6" t="n">
         <f aca="false">G21+C26</f>
@@ -800,14 +956,14 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B27" s="5" t="n">
         <f aca="false">B7</f>
         <v>21.2328767123288</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F27" s="6" t="n">
         <f aca="false">B27</f>
@@ -820,7 +976,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B28" s="11" t="n">
         <f aca="false">SUM(B25:B27)</f>
@@ -831,10 +987,14 @@
         <v>21.2328767123288</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H28" s="2" t="n">
         <f aca="false">H25+H26</f>
+        <v>603.767123287671</v>
+      </c>
+      <c r="I28" s="12" t="n">
+        <f aca="false">C7</f>
         <v>603.767123287671</v>
       </c>
     </row>
@@ -845,10 +1005,10 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F30" s="6" t="n">
         <f aca="false">$B$2</f>
@@ -865,7 +1025,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B31" s="6" t="n">
         <f aca="false">B9</f>
@@ -873,7 +1033,7 @@
       </c>
       <c r="C31" s="6"/>
       <c r="E31" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G31" s="6" t="n">
         <f aca="false">G26</f>
@@ -886,7 +1046,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B32" s="6"/>
       <c r="C32" s="6" t="n">
@@ -894,7 +1054,7 @@
         <v>1400</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F32" s="6" t="n">
         <f aca="false">B32</f>
@@ -907,7 +1067,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B33" s="11" t="n">
         <f aca="false">SUM(B30:B32)</f>
@@ -917,10 +1077,12 @@
         <f aca="false">SUM(C30:C32)</f>
         <v>1400</v>
       </c>
-      <c r="E33" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H33" s="2" t="n">
+      <c r="E33" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F33" s="14"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="15" t="n">
         <f aca="false">H30+H31</f>
         <v>-796.232876712329</v>
       </c>
@@ -930,7 +1092,7 @@
         <v>18</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F35" s="6" t="n">
         <f aca="false">F30+B36</f>
@@ -947,7 +1109,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B36" s="6" t="n">
         <f aca="false">B10-G26</f>
@@ -955,7 +1117,7 @@
       </c>
       <c r="C36" s="6"/>
       <c r="E36" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F36" s="6" t="n">
         <f aca="false">F26+B38</f>
@@ -980,7 +1142,7 @@
         <v>796.232876712329</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F37" s="6" t="n">
         <f aca="false">B37</f>
@@ -993,7 +1155,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B38" s="6" t="n">
         <f aca="false">G26</f>
@@ -1015,23 +1177,27 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B39" s="6"/>
       <c r="C39" s="6" t="n">
         <v>0</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H39" s="2" t="n">
         <f aca="false">H35+H36</f>
         <v>0</v>
       </c>
+      <c r="I39" s="12" t="n">
+        <f aca="false">C8</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B40" s="11" t="n">
         <f aca="false">SUM(B35:B39)</f>
@@ -1045,12 +1211,12 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B43" s="6"/>
       <c r="C43" s="6" t="n">
@@ -1058,7 +1224,7 @@
         <v>1000</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F43" s="6" t="n">
         <f aca="false">F25</f>
@@ -1083,7 +1249,7 @@
         <v>796.232876712329</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F44" s="6" t="n">
         <f aca="false">F26+B45</f>
@@ -1100,7 +1266,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B45" s="6" t="n">
         <f aca="false">B38</f>
@@ -1108,7 +1274,7 @@
       </c>
       <c r="C45" s="6"/>
       <c r="E45" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F45" s="6" t="n">
         <v>0</v>
@@ -1120,7 +1286,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B46" s="6" t="n">
         <f aca="false">B9</f>
@@ -1132,7 +1298,7 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B47" s="11" t="n">
         <f aca="false">SUM(B42:B46)</f>
@@ -1157,7 +1323,7 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E48" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H48" s="2" t="n">
         <f aca="false">H43+H44</f>
@@ -1181,10 +1347,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ48"/>
+  <dimension ref="A1:AMJ49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D40" activeCellId="0" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1380,10 +1546,13 @@
       <c r="H13" s="0" t="s">
         <v>26</v>
       </c>
+      <c r="I13" s="0" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E14" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G14" s="6" t="n">
         <f aca="false">$B$2</f>
@@ -1396,10 +1565,10 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F15" s="6" t="n">
         <f aca="false">$B$2</f>
@@ -1412,14 +1581,14 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C16" s="6" t="n">
         <f aca="false">B4</f>
         <v>150.819672131148</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G16" s="6" t="n">
         <f aca="false">C16</f>
@@ -1432,14 +1601,14 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B17" s="5" t="n">
         <f aca="false">B4</f>
         <v>150.819672131148</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F17" s="6" t="n">
         <f aca="false">B17</f>
@@ -1452,7 +1621,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B18" s="11" t="n">
         <f aca="false">SUM(B15:B17)</f>
@@ -1463,12 +1632,16 @@
         <v>150.819672131148</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H18" s="2" t="n">
         <f aca="false">H15+H16</f>
         <v>2349.18032786885</v>
       </c>
+      <c r="I18" s="12" t="n">
+        <f aca="false">C4</f>
+        <v>2349.18032786885</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G19" s="6"/>
@@ -1476,10 +1649,10 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F20" s="6" t="n">
         <f aca="false">$B$2</f>
@@ -1492,14 +1665,14 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C21" s="6" t="n">
         <f aca="false">B5</f>
         <v>600</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G21" s="6" t="n">
         <f aca="false">G16+C21</f>
@@ -1512,14 +1685,14 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B22" s="5" t="n">
         <f aca="false">B5</f>
         <v>600</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F22" s="6" t="n">
         <f aca="false">B22</f>
@@ -1532,7 +1705,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B23" s="11" t="n">
         <f aca="false">SUM(B20:B22)</f>
@@ -1543,19 +1716,23 @@
         <v>600</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H23" s="2" t="n">
         <f aca="false">H20+H21</f>
         <v>1749.18032786885</v>
       </c>
+      <c r="I23" s="12" t="n">
+        <f aca="false">C5</f>
+        <v>1749.18032786885</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F25" s="6" t="n">
         <f aca="false">$B$2</f>
@@ -1568,14 +1745,14 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C26" s="6" t="n">
         <f aca="false">B7</f>
         <v>50.958904109589</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G26" s="6" t="n">
         <f aca="false">G21+C26</f>
@@ -1588,14 +1765,14 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B27" s="5" t="n">
         <f aca="false">B7</f>
         <v>50.958904109589</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F27" s="6" t="n">
         <f aca="false">B27</f>
@@ -1608,7 +1785,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B28" s="11" t="n">
         <f aca="false">SUM(B25:B27)</f>
@@ -1619,10 +1796,14 @@
         <v>50.958904109589</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H28" s="2" t="n">
         <f aca="false">H25+H26</f>
+        <v>1698.22142375926</v>
+      </c>
+      <c r="I28" s="12" t="n">
+        <f aca="false">C7</f>
         <v>1698.22142375926</v>
       </c>
     </row>
@@ -1633,10 +1814,10 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F30" s="6" t="n">
         <f aca="false">$B$2</f>
@@ -1653,7 +1834,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B31" s="6" t="n">
         <f aca="false">B9</f>
@@ -1661,7 +1842,7 @@
       </c>
       <c r="C31" s="6"/>
       <c r="E31" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G31" s="6" t="n">
         <f aca="false">G26</f>
@@ -1674,7 +1855,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B32" s="6"/>
       <c r="C32" s="6" t="n">
@@ -1682,7 +1863,7 @@
         <v>3210</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F32" s="6" t="n">
         <f aca="false">B32</f>
@@ -1695,7 +1876,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B33" s="11" t="n">
         <f aca="false">SUM(B30:B32)</f>
@@ -1705,10 +1886,12 @@
         <f aca="false">SUM(C30:C32)</f>
         <v>3210</v>
       </c>
-      <c r="E33" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H33" s="2" t="n">
+      <c r="E33" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F33" s="14"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="15" t="n">
         <f aca="false">H30+H31</f>
         <v>-1511.77857624074</v>
       </c>
@@ -1718,7 +1901,7 @@
         <v>18</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F35" s="6" t="n">
         <f aca="false">F30+B36</f>
@@ -1735,7 +1918,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B36" s="6" t="n">
         <f aca="false">B10-G26</f>
@@ -1743,7 +1926,7 @@
       </c>
       <c r="C36" s="6"/>
       <c r="E36" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F36" s="6" t="n">
         <f aca="false">F26+B38</f>
@@ -1768,7 +1951,7 @@
         <v>1511.77857624074</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F37" s="6" t="n">
         <f aca="false">B37</f>
@@ -1781,7 +1964,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B38" s="6" t="n">
         <f aca="false">G26</f>
@@ -1803,23 +1986,27 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B39" s="6"/>
       <c r="C39" s="6" t="n">
         <v>0</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H39" s="2" t="n">
         <f aca="false">H35+H36</f>
         <v>0</v>
       </c>
+      <c r="I39" s="12" t="n">
+        <f aca="false">C8</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B40" s="11" t="n">
         <f aca="false">SUM(B35:B39)</f>
@@ -1831,124 +2018,145 @@
       </c>
       <c r="H40" s="6"/>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
-        <v>39</v>
-      </c>
-    </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="B43" s="6"/>
-      <c r="C43" s="6" t="n">
+      <c r="A43" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B43" s="16"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="16"/>
+      <c r="G43" s="16"/>
+      <c r="H43" s="16"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B44" s="17"/>
+      <c r="C44" s="17" t="n">
         <f aca="false">C32-B36</f>
         <v>2500</v>
       </c>
-      <c r="E43" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="F43" s="6" t="n">
+      <c r="D44" s="16"/>
+      <c r="E44" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="F44" s="17" t="n">
         <f aca="false">F25</f>
         <v>2500</v>
       </c>
-      <c r="G43" s="6" t="n">
-        <f aca="false">G25+C43</f>
+      <c r="G44" s="17" t="n">
+        <f aca="false">G25+C44</f>
         <v>2500</v>
       </c>
-      <c r="H43" s="6" t="n">
-        <f aca="false">F43-G43</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+      <c r="H44" s="17" t="n">
+        <f aca="false">F44-G44</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B44" s="6"/>
-      <c r="C44" s="5" t="n">
+      <c r="B45" s="17"/>
+      <c r="C45" s="18" t="n">
         <f aca="false">C37</f>
         <v>1511.77857624074</v>
       </c>
-      <c r="E44" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="F44" s="6" t="n">
-        <f aca="false">F26+B45</f>
+      <c r="D45" s="16"/>
+      <c r="E45" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="F45" s="17" t="n">
+        <f aca="false">F26+B46</f>
         <v>801.778576240737</v>
       </c>
-      <c r="G44" s="6" t="n">
+      <c r="G45" s="17" t="n">
         <f aca="false">G26</f>
         <v>801.778576240737</v>
       </c>
-      <c r="H44" s="6" t="n">
-        <f aca="false">F44-G44</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="B45" s="6" t="n">
+      <c r="H45" s="17" t="n">
+        <f aca="false">F45-G45</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B46" s="17" t="n">
         <f aca="false">B38</f>
         <v>801.778576240737</v>
       </c>
-      <c r="C45" s="6"/>
-      <c r="E45" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="F45" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H45" s="6" t="n">
-        <f aca="false">F45-G45</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="B46" s="6" t="n">
+      <c r="C46" s="17"/>
+      <c r="D46" s="16"/>
+      <c r="E46" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F46" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="G46" s="16"/>
+      <c r="H46" s="17" t="n">
+        <f aca="false">F46-G46</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B47" s="17" t="n">
         <f aca="false">B9</f>
         <v>3210</v>
       </c>
-      <c r="C46" s="6"/>
-      <c r="F46" s="6"/>
-      <c r="H46" s="6"/>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B47" s="11" t="n">
-        <f aca="false">SUM(B42:B46)</f>
+      <c r="C47" s="17"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="17"/>
+      <c r="G47" s="16"/>
+      <c r="H47" s="17"/>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B48" s="20" t="n">
+        <f aca="false">SUM(B43:B47)</f>
         <v>4011.77857624074</v>
       </c>
-      <c r="C47" s="11" t="n">
-        <f aca="false">SUM(C42:C46)</f>
+      <c r="C48" s="20" t="n">
+        <f aca="false">SUM(C43:C47)</f>
         <v>4011.77857624074</v>
       </c>
-      <c r="E47" s="0" t="s">
+      <c r="D48" s="16"/>
+      <c r="E48" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="F47" s="6"/>
-      <c r="G47" s="6" t="n">
-        <f aca="false">C44</f>
+      <c r="F48" s="17"/>
+      <c r="G48" s="17" t="n">
+        <f aca="false">C45</f>
         <v>1511.77857624074</v>
       </c>
-      <c r="H47" s="6" t="n">
-        <f aca="false">F47-G47</f>
+      <c r="H48" s="17" t="n">
+        <f aca="false">F48-G48</f>
         <v>-1511.77857624074</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E48" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H48" s="2" t="n">
-        <f aca="false">H43+H44</f>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="16"/>
+      <c r="B49" s="16"/>
+      <c r="C49" s="16"/>
+      <c r="D49" s="16"/>
+      <c r="E49" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="F49" s="16"/>
+      <c r="G49" s="16"/>
+      <c r="H49" s="22" t="n">
+        <f aca="false">H44+H45</f>
         <v>0</v>
       </c>
     </row>
@@ -1969,10 +2177,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ49"/>
+  <dimension ref="A1:AMJ37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1995,7 +2203,9 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2"/>
+      <c r="D1" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
@@ -2014,7 +2224,10 @@
         <f aca="false">B2</f>
         <v>1000</v>
       </c>
-      <c r="D2" s="6"/>
+      <c r="D2" s="6" t="n">
+        <f aca="false">B2</f>
+        <v>1000</v>
+      </c>
       <c r="F2" s="0" t="s">
         <v>5</v>
       </c>
@@ -2065,14 +2278,14 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B5" s="8" t="n">
-        <v>31</v>
+        <v>90</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="6"/>
-      <c r="G5" s="9"/>
+      <c r="G5" s="23"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
@@ -2080,678 +2293,513 @@
       </c>
       <c r="B6" s="5" t="n">
         <f aca="false">$G$3*B5/365</f>
-        <v>21.2328767123288</v>
+        <v>61.6438356164384</v>
       </c>
       <c r="C6" s="5" t="n">
         <f aca="false">C4-B6</f>
-        <v>853.767123287671</v>
+        <v>813.356164383562</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="0" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="8" t="n">
-        <v>31</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>15</v>
+        <v>45</v>
+      </c>
+      <c r="B7" s="4" t="n">
+        <v>725</v>
+      </c>
+      <c r="C7" s="5" t="n">
+        <f aca="false">C6-B7</f>
+        <v>88.3561643835617</v>
+      </c>
+      <c r="D7" s="6" t="n">
+        <f aca="false">D2-B7</f>
+        <v>275</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="G7" s="6" t="n">
+        <f aca="false">D7*G2</f>
+        <v>68.75</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="5" t="n">
-        <f aca="false">$G$3*B7/365</f>
-        <v>21.2328767123288</v>
-      </c>
-      <c r="C8" s="5" t="n">
-        <f aca="false">C6-B8</f>
-        <v>832.534246575342</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>17</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="B8" s="24" t="n">
+        <f aca="false">365-B5</f>
+        <v>275</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="6"/>
+      <c r="G8" s="25"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="B9" s="5" t="n">
-        <f aca="false">C8*$G$4</f>
-        <v>832.534246575342</v>
+        <f aca="false">$G$7*B8/365</f>
+        <v>51.7979452054795</v>
       </c>
       <c r="C9" s="5" t="n">
-        <f aca="false">C8-B9</f>
-        <v>0</v>
-      </c>
+        <f aca="false">C7-B9</f>
+        <v>36.5582191780822</v>
+      </c>
+      <c r="D9" s="6"/>
       <c r="E9" s="0" t="s">
-        <v>2</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="4" t="n">
-        <v>1400</v>
+        <v>14</v>
+      </c>
+      <c r="B10" s="8" t="n">
+        <v>31</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B11" s="5" t="n">
-        <f aca="false">B10-B9</f>
-        <v>567.465753424658</v>
+        <f aca="false">$G$7*B10/365</f>
+        <v>5.83904109589041</v>
+      </c>
+      <c r="C11" s="5" t="n">
+        <f aca="false">C9-B11</f>
+        <v>30.7191780821918</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>22</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="5" t="n">
+        <f aca="false">C11*$G$4</f>
+        <v>30.7191780821918</v>
+      </c>
+      <c r="C12" s="5" t="n">
+        <f aca="false">C11-B12</f>
+        <v>0</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D13" s="6"/>
+      <c r="A13" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="4" t="n">
+        <v>1400</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="5" t="n">
+        <f aca="false">B13-B12</f>
+        <v>1369.28082191781</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D16" s="6"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B17" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C17" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="F14" s="0" t="s">
+      <c r="F17" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="0" t="s">
+      <c r="G17" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="H14" s="0" t="s">
+      <c r="H17" s="0" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E15" s="0" t="s">
+      <c r="I17" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="G15" s="6" t="n">
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E18" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="G18" s="6" t="n">
         <f aca="false">$B$2</f>
         <v>1000</v>
       </c>
-      <c r="H15" s="6" t="n">
-        <f aca="false">F15-G15</f>
+      <c r="H18" s="6" t="n">
+        <f aca="false">F18-G18</f>
         <v>-1000</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" s="0" t="s">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="F16" s="6" t="n">
+      <c r="E19" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" s="6" t="n">
         <f aca="false">$B$2</f>
         <v>1000</v>
       </c>
-      <c r="H16" s="6" t="n">
-        <f aca="false">F16-G16</f>
+      <c r="H19" s="6" t="n">
+        <f aca="false">F19-G19</f>
         <v>1000</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="6" t="n">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="6" t="n">
         <f aca="false">B4</f>
         <v>125</v>
       </c>
-      <c r="E17" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="G17" s="6" t="n">
-        <f aca="false">C17</f>
+      <c r="E20" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="G20" s="6" t="n">
+        <f aca="false">C20</f>
         <v>125</v>
       </c>
-      <c r="H17" s="6" t="n">
-        <f aca="false">F17-G17</f>
+      <c r="H20" s="6" t="n">
+        <f aca="false">F20-G20</f>
         <v>-125</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" s="5" t="n">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="5" t="n">
         <f aca="false">B4</f>
         <v>125</v>
       </c>
-      <c r="E18" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="F18" s="6" t="n">
-        <f aca="false">B18</f>
+      <c r="E21" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="F21" s="6" t="n">
+        <f aca="false">B21</f>
         <v>125</v>
-      </c>
-      <c r="H18" s="6" t="n">
-        <f aca="false">F18-G18</f>
-        <v>125</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" s="11" t="n">
-        <f aca="false">SUM(B16:B18)</f>
-        <v>125</v>
-      </c>
-      <c r="C19" s="11" t="n">
-        <f aca="false">SUM(C16:C18)</f>
-        <v>125</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H19" s="2" t="n">
-        <f aca="false">H16+H17</f>
-        <v>875</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="E21" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="F21" s="6" t="n">
-        <f aca="false">$B$2</f>
-        <v>1000</v>
       </c>
       <c r="H21" s="6" t="n">
         <f aca="false">F21-G21</f>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="11" t="n">
+        <f aca="false">SUM(B19:B21)</f>
+        <v>125</v>
+      </c>
+      <c r="C22" s="11" t="n">
+        <f aca="false">SUM(C19:C21)</f>
+        <v>125</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H22" s="2" t="n">
+        <f aca="false">H19+H20</f>
+        <v>875</v>
+      </c>
+      <c r="I22" s="12" t="n">
+        <f aca="false">C4</f>
+        <v>875</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="F24" s="6" t="n">
+        <f aca="false">F19</f>
         <v>1000</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22" s="6" t="n">
+      <c r="H24" s="6" t="n">
+        <f aca="false">F24-G24</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="6" t="n">
         <f aca="false">B6</f>
-        <v>21.2328767123288</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="G22" s="6" t="n">
-        <f aca="false">G17+C22</f>
-        <v>146.232876712329</v>
-      </c>
-      <c r="H22" s="6" t="n">
-        <f aca="false">F22-G22</f>
-        <v>-146.232876712329</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23" s="5" t="n">
-        <f aca="false">B6</f>
-        <v>21.2328767123288</v>
-      </c>
-      <c r="E23" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="F23" s="6" t="n">
-        <f aca="false">B23</f>
-        <v>21.2328767123288</v>
-      </c>
-      <c r="H23" s="6" t="n">
-        <f aca="false">F23-G23</f>
-        <v>21.2328767123288</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B24" s="11" t="n">
-        <f aca="false">SUM(B21:B23)</f>
-        <v>21.2328767123288</v>
-      </c>
-      <c r="C24" s="11" t="n">
-        <f aca="false">SUM(C21:C23)</f>
-        <v>21.2328767123288</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H24" s="2" t="n">
-        <f aca="false">H21+H22</f>
-        <v>853.767123287671</v>
+        <v>61.6438356164384</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="G25" s="6" t="n">
+        <f aca="false">G20+C25</f>
+        <v>186.643835616438</v>
+      </c>
+      <c r="H25" s="6" t="n">
+        <f aca="false">F25-G25</f>
+        <v>-186.643835616438</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>36</v>
+        <v>32</v>
+      </c>
+      <c r="B26" s="5" t="n">
+        <f aca="false">B6</f>
+        <v>61.6438356164384</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F26" s="6" t="n">
-        <f aca="false">$B$2</f>
-        <v>1000</v>
+        <f aca="false">B26</f>
+        <v>61.6438356164384</v>
       </c>
       <c r="H26" s="6" t="n">
         <f aca="false">F26-G26</f>
+        <v>61.6438356164384</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="11" t="n">
+        <f aca="false">SUM(B24:B26)</f>
+        <v>61.6438356164384</v>
+      </c>
+      <c r="C27" s="11" t="n">
+        <f aca="false">SUM(C24:C26)</f>
+        <v>61.6438356164384</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H27" s="2" t="n">
+        <f aca="false">H24+H25</f>
+        <v>813.356164383562</v>
+      </c>
+      <c r="I27" s="12" t="n">
+        <f aca="false">C6</f>
+        <v>813.356164383562</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="F29" s="6" t="n">
+        <f aca="false">F24</f>
         <v>1000</v>
       </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="G29" s="6" t="n">
+        <f aca="false">C30</f>
+        <v>725</v>
+      </c>
+      <c r="H29" s="6" t="n">
+        <f aca="false">F29-G29</f>
+        <v>275</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="6" t="n">
-        <f aca="false">B8</f>
-        <v>21.2328767123288</v>
-      </c>
-      <c r="E27" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="G27" s="6" t="n">
-        <f aca="false">G22+C27</f>
-        <v>167.465753424658</v>
-      </c>
-      <c r="H27" s="6" t="n">
-        <f aca="false">F27-G27</f>
-        <v>-167.465753424658</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="B28" s="5" t="n">
-        <f aca="false">B8</f>
-        <v>21.2328767123288</v>
-      </c>
-      <c r="E28" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="F28" s="6" t="n">
-        <f aca="false">B28</f>
-        <v>21.2328767123288</v>
-      </c>
-      <c r="H28" s="6" t="n">
-        <f aca="false">F28-G28</f>
-        <v>21.2328767123288</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B29" s="11" t="n">
-        <f aca="false">SUM(B26:B28)</f>
-        <v>21.2328767123288</v>
-      </c>
-      <c r="C29" s="11" t="n">
-        <f aca="false">SUM(C26:C28)</f>
-        <v>21.2328767123288</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H29" s="2" t="n">
-        <f aca="false">H26+H27</f>
-        <v>832.534246575342</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="10"/>
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
+      <c r="C30" s="6" t="n">
+        <f aca="false">B7</f>
+        <v>725</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="G30" s="6" t="n">
+        <f aca="false">G25</f>
+        <v>186.643835616438</v>
+      </c>
+      <c r="H30" s="6" t="n">
+        <f aca="false">F30-G30</f>
+        <v>-186.643835616438</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>37</v>
+        <v>50</v>
+      </c>
+      <c r="B31" s="26" t="n">
+        <f aca="false">B7</f>
+        <v>725</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F31" s="6" t="n">
-        <f aca="false">$B$2</f>
-        <v>1000</v>
-      </c>
-      <c r="G31" s="6" t="n">
-        <f aca="false">C33</f>
-        <v>1400</v>
+        <f aca="false">F26</f>
+        <v>61.6438356164384</v>
       </c>
       <c r="H31" s="6" t="n">
         <f aca="false">F31-G31</f>
-        <v>-400</v>
+        <v>61.6438356164384</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="B32" s="6" t="n">
-        <f aca="false">B10</f>
-        <v>1400</v>
-      </c>
-      <c r="C32" s="6"/>
-      <c r="E32" s="0" t="s">
+      <c r="A32" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" s="11" t="n">
+        <f aca="false">SUM(B29:B31)</f>
+        <v>725</v>
+      </c>
+      <c r="C32" s="11" t="n">
+        <f aca="false">SUM(C29:C31)</f>
+        <v>725</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H32" s="2" t="n">
+        <f aca="false">H29+H30</f>
+        <v>88.3561643835616</v>
+      </c>
+      <c r="I32" s="12" t="n">
+        <f aca="false">C7</f>
+        <v>88.3561643835617</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="10"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="E34" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="G32" s="6" t="n">
-        <f aca="false">G27</f>
-        <v>167.465753424658</v>
-      </c>
-      <c r="H32" s="6" t="n">
-        <f aca="false">F32-G32</f>
-        <v>-167.465753424658</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6" t="n">
-        <f aca="false">B10</f>
-        <v>1400</v>
-      </c>
-      <c r="E33" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="F33" s="6" t="n">
-        <f aca="false">B33</f>
-        <v>0</v>
-      </c>
-      <c r="H33" s="6" t="n">
-        <f aca="false">F33-G33</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B34" s="11" t="n">
-        <f aca="false">SUM(B31:B33)</f>
-        <v>1400</v>
-      </c>
-      <c r="C34" s="11" t="n">
-        <f aca="false">SUM(C31:C33)</f>
-        <v>1400</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H34" s="2" t="n">
-        <f aca="false">H31+H32</f>
-        <v>-567.465753424658</v>
+      <c r="F34" s="6" t="n">
+        <f aca="false">F29</f>
+        <v>1000</v>
+      </c>
+      <c r="G34" s="6" t="n">
+        <f aca="false">G29</f>
+        <v>725</v>
+      </c>
+      <c r="H34" s="6" t="n">
+        <f aca="false">F34-G34</f>
+        <v>275</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C35" s="6" t="n">
+        <f aca="false">B9</f>
+        <v>51.7979452054795</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="G35" s="6" t="n">
+        <f aca="false">G30+C35</f>
+        <v>238.441780821918</v>
+      </c>
+      <c r="H35" s="6" t="n">
+        <f aca="false">F35-G35</f>
+        <v>-238.441780821918</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>18</v>
+        <v>32</v>
+      </c>
+      <c r="B36" s="5" t="n">
+        <f aca="false">B9</f>
+        <v>51.7979452054795</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F36" s="6" t="n">
-        <f aca="false">F31+B37</f>
-        <v>1400</v>
-      </c>
-      <c r="G36" s="6" t="n">
-        <f aca="false">G31+C40</f>
-        <v>1400</v>
+        <f aca="false">F31+B36</f>
+        <v>113.441780821918</v>
       </c>
       <c r="H36" s="6" t="n">
         <f aca="false">F36-G36</f>
-        <v>0</v>
+        <v>113.441780821918</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="B37" s="6" t="n">
-        <f aca="false">B11-G27</f>
-        <v>400</v>
-      </c>
-      <c r="C37" s="6"/>
-      <c r="E37" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="F37" s="6" t="n">
-        <f aca="false">F27+B39</f>
-        <v>167.465753424658</v>
-      </c>
-      <c r="G37" s="6" t="n">
-        <f aca="false">G27</f>
-        <v>167.465753424658</v>
-      </c>
-      <c r="H37" s="6" t="n">
-        <f aca="false">F37-G37</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="B38" s="6"/>
-      <c r="C38" s="5" t="n">
-        <f aca="false">B11</f>
-        <v>567.465753424658</v>
-      </c>
-      <c r="E38" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="F38" s="6" t="n">
-        <f aca="false">B38</f>
-        <v>0</v>
-      </c>
-      <c r="H38" s="6" t="n">
-        <f aca="false">F38-G38</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="B39" s="6" t="n">
-        <f aca="false">G27</f>
-        <v>167.465753424658</v>
-      </c>
-      <c r="C39" s="6"/>
-      <c r="E39" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6" t="n">
-        <f aca="false">C38</f>
-        <v>567.465753424658</v>
-      </c>
-      <c r="H39" s="6" t="n">
-        <f aca="false">F39-G39</f>
-        <v>-567.465753424658</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="B40" s="6"/>
-      <c r="C40" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E40" s="1" t="s">
+      <c r="A37" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="H40" s="2" t="n">
-        <f aca="false">H36+H37</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B41" s="11" t="n">
-        <f aca="false">SUM(B36:B40)</f>
-        <v>567.465753424658</v>
-      </c>
-      <c r="C41" s="11" t="n">
-        <f aca="false">SUM(C36:C40)</f>
-        <v>567.465753424658</v>
-      </c>
-      <c r="H41" s="6"/>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="B44" s="6"/>
-      <c r="C44" s="6" t="n">
-        <f aca="false">C33-B37</f>
-        <v>1000</v>
-      </c>
-      <c r="E44" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="F44" s="6" t="n">
-        <f aca="false">F26</f>
-        <v>1000</v>
-      </c>
-      <c r="G44" s="6" t="n">
-        <f aca="false">G26+C44</f>
-        <v>1000</v>
-      </c>
-      <c r="H44" s="6" t="n">
-        <f aca="false">F44-G44</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="B45" s="6"/>
-      <c r="C45" s="5" t="n">
-        <f aca="false">C38</f>
-        <v>567.465753424658</v>
-      </c>
-      <c r="E45" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="F45" s="6" t="n">
-        <f aca="false">F27+B46</f>
-        <v>167.465753424658</v>
-      </c>
-      <c r="G45" s="6" t="n">
-        <f aca="false">G27</f>
-        <v>167.465753424658</v>
-      </c>
-      <c r="H45" s="6" t="n">
-        <f aca="false">F45-G45</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="B46" s="6" t="n">
-        <f aca="false">B39</f>
-        <v>167.465753424658</v>
-      </c>
-      <c r="C46" s="6"/>
-      <c r="E46" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="F46" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H46" s="6" t="n">
-        <f aca="false">F46-G46</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="B47" s="6" t="n">
-        <f aca="false">B10</f>
-        <v>1400</v>
-      </c>
-      <c r="C47" s="6"/>
-      <c r="F47" s="6"/>
-      <c r="H47" s="6"/>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B48" s="11" t="n">
-        <f aca="false">SUM(B43:B47)</f>
-        <v>1567.46575342466</v>
-      </c>
-      <c r="C48" s="11" t="n">
-        <f aca="false">SUM(C43:C47)</f>
-        <v>1567.46575342466</v>
-      </c>
-      <c r="E48" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="F48" s="6"/>
-      <c r="G48" s="6" t="n">
-        <f aca="false">C45</f>
-        <v>567.465753424658</v>
-      </c>
-      <c r="H48" s="6" t="n">
-        <f aca="false">F48-G48</f>
-        <v>-567.465753424658</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E49" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H49" s="2" t="n">
-        <f aca="false">H44+H45</f>
-        <v>0</v>
+      <c r="B37" s="11" t="n">
+        <f aca="false">SUM(B34:B36)</f>
+        <v>51.7979452054795</v>
+      </c>
+      <c r="C37" s="11" t="n">
+        <f aca="false">SUM(C34:C36)</f>
+        <v>51.7979452054795</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H37" s="2" t="n">
+        <f aca="false">H34+H35</f>
+        <v>36.5582191780822</v>
+      </c>
+      <c r="I37" s="12" t="n">
+        <f aca="false">C9</f>
+        <v>36.5582191780822</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="true" objects="true" scenarios="true"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -2828,7 +2876,7 @@
         <v>92</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>8</v>
@@ -2852,7 +2900,7 @@
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="0" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>11</v>
@@ -2907,7 +2955,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="B8" s="5" t="n">
         <f aca="false">C7*$G$4</f>
@@ -2969,7 +3017,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E14" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G14" s="6" t="n">
         <f aca="false">$B$2</f>
@@ -2982,10 +3030,10 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F15" s="6" t="n">
         <f aca="false">$B$2</f>
@@ -2998,14 +3046,14 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C16" s="6" t="n">
         <f aca="false">B4</f>
         <v>150.819672131148</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G16" s="6" t="n">
         <f aca="false">C16</f>
@@ -3018,14 +3066,14 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B17" s="5" t="n">
         <f aca="false">B4</f>
         <v>150.819672131148</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F17" s="6" t="n">
         <f aca="false">B17</f>
@@ -3038,7 +3086,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B18" s="11" t="n">
         <f aca="false">SUM(B15:B17)</f>
@@ -3049,7 +3097,7 @@
         <v>150.819672131148</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H18" s="2" t="n">
         <f aca="false">H15+H16</f>
@@ -3062,10 +3110,10 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F20" s="6" t="n">
         <f aca="false">$B$2</f>
@@ -3078,14 +3126,14 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C21" s="6" t="n">
         <f aca="false">B5</f>
         <v>600</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G21" s="6" t="n">
         <f aca="false">G16+C21</f>
@@ -3098,14 +3146,14 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B22" s="5" t="n">
         <f aca="false">B5</f>
         <v>600</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F22" s="6" t="n">
         <f aca="false">B22</f>
@@ -3118,7 +3166,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B23" s="11" t="n">
         <f aca="false">SUM(B20:B22)</f>
@@ -3129,7 +3177,7 @@
         <v>600</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H23" s="2" t="n">
         <f aca="false">H20+H21</f>
@@ -3138,10 +3186,10 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F25" s="6" t="n">
         <f aca="false">$B$2</f>
@@ -3154,14 +3202,14 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C26" s="6" t="n">
         <f aca="false">B7</f>
         <v>348.493150684931</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G26" s="6" t="n">
         <f aca="false">G21+C26</f>
@@ -3174,14 +3222,14 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B27" s="5" t="n">
         <f aca="false">B7</f>
         <v>348.493150684931</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F27" s="6" t="n">
         <f aca="false">B27</f>
@@ -3194,7 +3242,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B28" s="11" t="n">
         <f aca="false">SUM(B25:B27)</f>
@@ -3205,7 +3253,7 @@
         <v>348.493150684931</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H28" s="2" t="n">
         <f aca="false">H25+H26</f>
@@ -3219,10 +3267,10 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F30" s="6" t="n">
         <f aca="false">$B$2</f>
@@ -3239,7 +3287,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B31" s="6" t="n">
         <f aca="false">B9</f>
@@ -3247,7 +3295,7 @@
       </c>
       <c r="C31" s="6"/>
       <c r="E31" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G31" s="6" t="n">
         <f aca="false">G26</f>
@@ -3260,7 +3308,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B32" s="6"/>
       <c r="C32" s="6" t="n">
@@ -3268,7 +3316,7 @@
         <v>550</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F32" s="6" t="n">
         <f aca="false">B32</f>
@@ -3281,7 +3329,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B33" s="11" t="n">
         <f aca="false">SUM(B30:B32)</f>
@@ -3292,7 +3340,7 @@
         <v>550</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H33" s="2" t="n">
         <f aca="false">H30+H31</f>
@@ -3305,7 +3353,7 @@
         <v>18</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F35" s="6" t="n">
         <f aca="false">F30+B36</f>
@@ -3322,7 +3370,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B36" s="6" t="n">
         <f aca="false">B10-G26*G4</f>
@@ -3330,7 +3378,7 @@
       </c>
       <c r="C36" s="6"/>
       <c r="E36" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F36" s="6" t="n">
         <f aca="false">F26+B38</f>
@@ -3355,7 +3403,7 @@
         <v>269.862564563216</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F37" s="6" t="n">
         <f aca="false">B37</f>
@@ -3368,7 +3416,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B38" s="6" t="n">
         <f aca="false">G26*G4</f>
@@ -3390,14 +3438,14 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B39" s="6"/>
       <c r="C39" s="6" t="n">
         <v>0</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H39" s="2" t="n">
         <f aca="false">H35+H36</f>
@@ -3406,7 +3454,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B40" s="11" t="n">
         <f aca="false">SUM(B35:B39)</f>
@@ -3419,12 +3467,12 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B43" s="6"/>
       <c r="C43" s="6" t="n">
@@ -3432,7 +3480,7 @@
         <v>500</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F43" s="6" t="n">
         <f aca="false">F25</f>
@@ -3457,7 +3505,7 @@
         <v>269.862564563216</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F44" s="6" t="n">
         <f aca="false">F26+B45</f>
@@ -3474,7 +3522,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B45" s="6" t="n">
         <f aca="false">B38</f>
@@ -3482,7 +3530,7 @@
       </c>
       <c r="C45" s="6"/>
       <c r="E45" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F45" s="6" t="n">
         <v>0</v>
@@ -3494,7 +3542,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B46" s="6" t="n">
         <f aca="false">B9</f>
@@ -3506,7 +3554,7 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B47" s="11" t="n">
         <f aca="false">SUM(B42:B46)</f>
@@ -3531,7 +3579,7 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E48" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H48" s="2" t="n">
         <f aca="false">H43+H44</f>
@@ -3539,7 +3587,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="true" objects="true" scenarios="true"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>